<commit_message>
Backlog done code still has errors!!!
Still trying to fix the code but the sprint backlog part is done.
</commit_message>
<xml_diff>
--- a/SnakeGame/Documents/Backlog Doc.xlsx
+++ b/SnakeGame/Documents/Backlog Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztllo\OneDrive\Documents\GitHub\SnakeGame\SnakeGame\SnakeGame\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justy\source\repos\SnakeGame\SnakeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C680CF3A-3E18-4D3F-B45D-A70203AC7576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F83855C1-27BA-495C-A281-E0613C370E59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
+    <workbookView xWindow="14028" yWindow="5052" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
   <si>
     <t>Time Spent</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Start adding in buttons for the menu and GUI</t>
+  </si>
+  <si>
+    <t>Summary</t>
   </si>
 </sst>
 </file>
@@ -385,7 +388,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -420,11 +423,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -437,13 +447,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -470,11 +477,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -821,76 +825,76 @@
       <selection activeCell="A13" sqref="A13:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="73.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
-    <col min="15" max="16" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="73.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="5" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="16" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A2" s="22"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="23"/>
+      <c r="P3" s="23"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -940,7 +944,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -980,7 +984,7 @@
       </c>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1018,7 +1022,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1056,7 +1060,7 @@
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1098,7 +1102,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1146,132 +1150,132 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="25"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="K13" s="25"/>
+      <c r="L13" s="25"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="19"/>
+      <c r="I15" s="19"/>
+      <c r="J15" s="19"/>
+      <c r="K15" s="19"/>
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="19"/>
+      <c r="J17" s="19"/>
+      <c r="K17" s="19"/>
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="19"/>
+      <c r="E19" s="19"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19"/>
+      <c r="I19" s="19"/>
+      <c r="J19" s="19"/>
+      <c r="K19" s="19"/>
+      <c r="L19" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="A13:N13"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C18:L18"/>
-    <mergeCell ref="A1:P2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="A13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1292,29 +1296,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2156A0E-8028-4373-98BC-103EF4FEF8E3}">
-  <dimension ref="A1:Q29"/>
+  <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="68.28515625" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="2" max="2" width="68.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="9" width="7.7109375" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="17.85546875" customWidth="1"/>
-    <col min="13" max="13" width="20.28515625" customWidth="1"/>
-    <col min="14" max="14" width="18.140625" customWidth="1"/>
-    <col min="15" max="15" width="16.85546875" customWidth="1"/>
+    <col min="8" max="9" width="7.6640625" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" customWidth="1"/>
+    <col min="12" max="12" width="17.88671875" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" customWidth="1"/>
+    <col min="14" max="14" width="18.109375" customWidth="1"/>
+    <col min="15" max="15" width="16.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1330,7 +1334,7 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="28" t="s">
         <v>31</v>
       </c>
@@ -1349,7 +1353,7 @@
       <c r="N2" s="29"/>
       <c r="O2" s="29"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
         <v>32</v>
       </c>
@@ -1368,7 +1372,7 @@
       <c r="N3" s="31"/>
       <c r="O3" s="31"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="32" t="s">
         <v>33</v>
       </c>
@@ -1387,7 +1391,7 @@
       <c r="N4" s="33"/>
       <c r="O4" s="33"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1401,95 +1405,127 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-      <c r="N6" s="19"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="34" t="s">
+      <c r="M6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="3">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43738</v>
+      </c>
+      <c r="F7" s="3">
+        <v>5</v>
+      </c>
+      <c r="G7" s="3">
+        <v>5</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3">
+        <v>5</v>
+      </c>
+      <c r="K7" s="18">
+        <v>43740</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>1.1000000000000001</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="3">
+        <v>41</v>
+      </c>
+      <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E8" s="5">
         <v>43738</v>
       </c>
       <c r="F8" s="3">
+        <v>15</v>
+      </c>
+      <c r="G8" s="3">
+        <v>10</v>
+      </c>
+      <c r="H8" s="3">
         <v>5</v>
       </c>
-      <c r="G8" s="3">
-        <v>5</v>
-      </c>
-      <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="20">
+      <c r="J8" s="3">
+        <v>15</v>
+      </c>
+      <c r="K8" s="18">
         <v>43740</v>
       </c>
       <c r="L8" s="3" t="s">
@@ -1504,15 +1540,13 @@
       <c r="O8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P8" s="25"/>
-      <c r="Q8" s="25"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -1527,35 +1561,33 @@
         <v>10</v>
       </c>
       <c r="G9" s="3">
+        <v>5</v>
+      </c>
+      <c r="H9" s="3">
         <v>10</v>
       </c>
-      <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
-      <c r="K9" s="20">
-        <v>43740</v>
+      <c r="K9" s="5">
+        <v>43749</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O9" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>1.2</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="4">
+        <v>49</v>
+      </c>
+      <c r="C10" s="3">
         <v>1</v>
       </c>
       <c r="D10" s="3">
@@ -1568,27 +1600,35 @@
         <v>5</v>
       </c>
       <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
+      <c r="H10" s="3">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>5</v>
+      </c>
+      <c r="J10" s="3">
+        <v>10</v>
+      </c>
+      <c r="K10" s="5">
+        <v>43756</v>
+      </c>
       <c r="L10" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>1.2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="3">
+        <v>51</v>
+      </c>
+      <c r="C11" s="4">
         <v>1</v>
       </c>
       <c r="D11" s="3">
@@ -1598,45 +1638,61 @@
         <v>43738</v>
       </c>
       <c r="F11" s="3">
-        <v>5</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="G11" s="3">
+        <v>6</v>
+      </c>
+      <c r="H11" s="3">
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>6</v>
+      </c>
+      <c r="J11" s="3">
+        <v>18</v>
+      </c>
+      <c r="K11" s="5">
+        <v>43756</v>
+      </c>
       <c r="L11" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="N11" s="6"/>
+      <c r="N11" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="4">
+        <v>52</v>
+      </c>
+      <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E12" s="5">
         <v>43738</v>
       </c>
       <c r="F12" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="I12" s="3">
+        <v>5</v>
+      </c>
+      <c r="J12" s="3">
+        <v>5</v>
+      </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
         <v>50</v>
@@ -1645,18 +1701,20 @@
         <v>28</v>
       </c>
       <c r="N12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="O12" s="6"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>1.3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="3">
+        <v>53</v>
+      </c>
+      <c r="C13" s="4">
         <v>1</v>
       </c>
       <c r="D13" s="3">
@@ -1666,32 +1724,34 @@
         <v>43738</v>
       </c>
       <c r="F13" s="3">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>3</v>
+      </c>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
         <v>50</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="O13" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O13" s="6"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>1.3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -1707,8 +1767,12 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>3</v>
+      </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
         <v>50</v>
@@ -1721,24 +1785,24 @@
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>1.3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="4">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E15" s="5">
         <v>43738</v>
       </c>
       <c r="F15" s="3">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -1756,12 +1820,12 @@
       </c>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>1.3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1791,42 +1855,24 @@
       </c>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1.3</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="3">
-        <v>1</v>
-      </c>
-      <c r="D17" s="3">
-        <v>3</v>
-      </c>
-      <c r="E17" s="5">
-        <v>43738</v>
-      </c>
-      <c r="F17" s="3">
-        <v>5</v>
-      </c>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>29</v>
-      </c>
+      <c r="L17" s="3"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1843,189 +1889,179 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="3"/>
-      <c r="K19" s="3"/>
-      <c r="L19" s="3"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="6"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="14">
+      <c r="E19" s="14">
         <v>43738</v>
       </c>
-      <c r="F20" s="11">
-        <v>85</v>
-      </c>
-      <c r="G20" s="11">
+      <c r="F19" s="11">
+        <v>110</v>
+      </c>
+      <c r="G19" s="11">
         <v>15</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="3" t="s">
+      <c r="H19" s="11">
+        <v>26</v>
+      </c>
+      <c r="I19" s="11">
+        <v>22</v>
+      </c>
+      <c r="J19" s="11">
+        <v>48</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="M20" s="13" t="s">
+      <c r="M19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="N20" s="13" t="s">
+      <c r="N19" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="O20" s="13" t="s">
+      <c r="O19" s="13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="24"/>
-      <c r="N23" s="24"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B22" s="25"/>
+      <c r="C22" s="25"/>
+      <c r="D22" s="25"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+      <c r="G22" s="25"/>
+      <c r="H22" s="25"/>
+      <c r="I22" s="25"/>
+      <c r="J22" s="25"/>
+      <c r="K22" s="25"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="25"/>
+      <c r="N22" s="25"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B23" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C23" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="27"/>
+      <c r="D26" s="27"/>
+      <c r="E26" s="27"/>
+      <c r="F26" s="27"/>
+      <c r="G26" s="27"/>
+      <c r="H26" s="27"/>
+      <c r="I26" s="27"/>
+      <c r="J26" s="27"/>
+      <c r="K26" s="27"/>
+      <c r="L26" s="27"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A27">
         <v>4</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>1</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>2</v>
-      </c>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="25"/>
-      <c r="J26" s="25"/>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>3</v>
-      </c>
-      <c r="C27" s="37"/>
-      <c r="D27" s="37"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
-      <c r="H27" s="37"/>
-      <c r="I27" s="37"/>
-      <c r="J27" s="37"/>
-      <c r="K27" s="37"/>
-      <c r="L27" s="37"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+      <c r="K27" s="26"/>
+      <c r="L27" s="26"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
-        <v>4</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
-      <c r="K28" s="36"/>
-      <c r="L28" s="36"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A29">
         <v>5</v>
       </c>
-      <c r="C29" s="25"/>
-      <c r="D29" s="25"/>
-      <c r="E29" s="25"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
-      <c r="L29" s="25"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="13">
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="C27:L27"/>
     <mergeCell ref="C28:L28"/>
-    <mergeCell ref="C29:L29"/>
-    <mergeCell ref="A23:N23"/>
+    <mergeCell ref="A22:N22"/>
+    <mergeCell ref="C23:L23"/>
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C25:L25"/>
     <mergeCell ref="C26:L26"/>
-    <mergeCell ref="C27:L27"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Sprint 2 Log added
</commit_message>
<xml_diff>
--- a/SnakeGame/Documents/Backlog Doc.xlsx
+++ b/SnakeGame/Documents/Backlog Doc.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztllo\OneDrive\Documents\GitHub\SnakeGame\SnakeGame\SnakeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{879C50E1-E054-49CA-81DA-AA014B3CA4D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363EBFD6-72F3-4FA0-A022-C3C82D24AC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
     <sheet name="Sprint 1 Backlog" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2 Backlog" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="67">
   <si>
     <t>Time Spent</t>
   </si>
@@ -208,6 +209,33 @@
   </si>
   <si>
     <t>Summary</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Not Completed</t>
+  </si>
+  <si>
+    <t>Sprint 2 Backlog</t>
+  </si>
+  <si>
+    <t>Start the functionality of the board/level by incorporating it into the class</t>
+  </si>
+  <si>
+    <t>Start the functionality of the snake by incorporating it into the class</t>
+  </si>
+  <si>
+    <t>Start the functionality of the game loop by incorporating it into the class</t>
+  </si>
+  <si>
+    <t>Start the functionality of the menu by incorporating it into the class</t>
+  </si>
+  <si>
+    <t>Finish implementing QT library to add a GUI to the project</t>
+  </si>
+  <si>
+    <t>Finish creating grahpical interface by using QT</t>
   </si>
 </sst>
 </file>
@@ -388,7 +416,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -428,6 +456,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -837,62 +868,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
+      <c r="A2" s="21"/>
+      <c r="B2" s="21"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21" t="s">
+      <c r="A3" s="22"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1151,22 +1182,22 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23"/>
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
+      <c r="K13" s="24"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1175,93 +1206,93 @@
       <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="27"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
+      <c r="K14" s="27"/>
+      <c r="L14" s="27"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1298,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2156A0E-8028-4373-98BC-103EF4FEF8E3}">
   <dimension ref="A1:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1335,61 +1366,61 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
-      <c r="J2" s="28"/>
-      <c r="K2" s="28"/>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="28"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
-      <c r="H3" s="30"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="30"/>
-      <c r="L3" s="30"/>
-      <c r="M3" s="30"/>
-      <c r="N3" s="30"/>
-      <c r="O3" s="30"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="32"/>
-      <c r="C4" s="32"/>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1405,8 +1436,8 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="32"/>
-      <c r="O5" s="32"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1445,11 +1476,11 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="33" t="s">
+      <c r="M6" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="34"/>
-      <c r="O6" s="34"/>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1497,8 +1528,8 @@
       <c r="O7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -1709,9 +1740,11 @@
       <c r="J12" s="3">
         <v>5</v>
       </c>
-      <c r="K12" s="3"/>
+      <c r="K12" s="5">
+        <v>43756</v>
+      </c>
       <c r="L12" s="3" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>28</v>
@@ -1754,7 +1787,9 @@
       <c r="J13" s="3">
         <v>15</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="K13" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="L13" s="3" t="s">
         <v>50</v>
       </c>
@@ -1797,7 +1832,9 @@
       <c r="J14" s="3">
         <v>15</v>
       </c>
-      <c r="K14" s="3"/>
+      <c r="K14" s="4" t="s">
+        <v>58</v>
+      </c>
       <c r="L14" s="3" t="s">
         <v>50</v>
       </c>
@@ -1842,7 +1879,7 @@
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>27</v>
@@ -1885,7 +1922,7 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>27</v>
@@ -1975,22 +2012,22 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
+      <c r="A22" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-      <c r="K22" s="23"/>
-      <c r="L22" s="23"/>
-      <c r="M22" s="23"/>
-      <c r="N22" s="23"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -1999,93 +2036,93 @@
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="24"/>
-      <c r="L28" s="24"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2106,4 +2143,690 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5EE9B2-143D-4149-A7B5-D0F1922FD7D1}">
+  <dimension ref="A1:O28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="33"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="35"/>
+      <c r="O6" s="35"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" s="4">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F9" s="3">
+        <v>15</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F10" s="3">
+        <v>15</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F11" s="3">
+        <v>15</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="O11" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F12" s="3">
+        <v>15</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M12" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="4">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>2</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F13" s="3">
+        <v>15</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="4">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F14" s="3">
+        <v>15</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>3</v>
+      </c>
+      <c r="E15" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F15" s="3">
+        <v>15</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M15" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43759</v>
+      </c>
+      <c r="F16" s="3">
+        <v>15</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="14">
+        <v>43738</v>
+      </c>
+      <c r="F19" s="11">
+        <v>120</v>
+      </c>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11"/>
+      <c r="L19" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="N19" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="24"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
+      <c r="K22" s="24"/>
+      <c r="L22" s="24"/>
+      <c r="M22" s="24"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="27"/>
+      <c r="E23" s="27"/>
+      <c r="F23" s="27"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="27"/>
+      <c r="K23" s="27"/>
+      <c r="L23" s="27"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="C24" s="25"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
+      <c r="G25" s="25"/>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="25"/>
+      <c r="L25" s="25"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3</v>
+      </c>
+      <c r="C26" s="37"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>4</v>
+      </c>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="25"/>
+      <c r="J28" s="25"/>
+      <c r="K28" s="25"/>
+      <c r="L28" s="25"/>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="C28:L28"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="A22:N22"/>
+    <mergeCell ref="C23:L23"/>
+    <mergeCell ref="C24:L24"/>
+    <mergeCell ref="C25:L25"/>
+    <mergeCell ref="C26:L26"/>
+    <mergeCell ref="C27:L27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates made to product backlog and sprint log 1
</commit_message>
<xml_diff>
--- a/SnakeGame/Documents/Backlog Doc.xlsx
+++ b/SnakeGame/Documents/Backlog Doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztllo\OneDrive\Documents\GitHub\SnakeGame\SnakeGame\SnakeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363EBFD6-72F3-4FA0-A022-C3C82D24AC25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{747AE4E6-7D10-4ED5-8BF7-3581DCEBF7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
   <si>
     <t>Time Spent</t>
   </si>
@@ -236,6 +236,15 @@
   </si>
   <si>
     <t>Finish creating grahpical interface by using QT</t>
+  </si>
+  <si>
+    <t>QT was unable to be implemented</t>
+  </si>
+  <si>
+    <t>With the lack of knowledge of implementing QT we decided to drop it and keep the application console based</t>
+  </si>
+  <si>
+    <t>Dropped</t>
   </si>
 </sst>
 </file>
@@ -416,7 +425,7 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -460,6 +469,15 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -472,13 +490,10 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -505,12 +520,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
@@ -853,7 +864,7 @@
   <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:N13"/>
+      <selection activeCell="C15" sqref="C15:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,62 +879,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22" t="s">
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="22"/>
-      <c r="O3" s="22"/>
-      <c r="P3" s="22"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1182,22 +1193,22 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24"/>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="24"/>
-      <c r="L13" s="24"/>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1206,107 +1217,112 @@
       <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27"/>
-      <c r="K14" s="27"/>
-      <c r="L14" s="27"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
+      <c r="B15" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
-      <c r="L19" s="25"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="A13:N13"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C18:L18"/>
-    <mergeCell ref="A1:P2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="A13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1330,7 +1346,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,61 +1382,61 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1436,8 +1452,8 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1476,11 +1492,11 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="M6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1528,8 +1544,8 @@
       <c r="O7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="25"/>
-      <c r="Q7" s="25"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -2012,22 +2028,22 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2036,96 +2052,107 @@
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="B24" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="C27:L27"/>
     <mergeCell ref="C28:L28"/>
     <mergeCell ref="A22:N22"/>
@@ -2133,12 +2160,6 @@
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C25:L25"/>
     <mergeCell ref="C26:L26"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2150,7 +2171,7 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2182,61 +2203,61 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
-      <c r="M2" s="29"/>
-      <c r="N2" s="29"/>
-      <c r="O2" s="29"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="31"/>
-      <c r="E3" s="31"/>
-      <c r="F3" s="31"/>
-      <c r="G3" s="31"/>
-      <c r="H3" s="31"/>
-      <c r="I3" s="31"/>
-      <c r="J3" s="31"/>
-      <c r="K3" s="31"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="31"/>
-      <c r="N3" s="31"/>
-      <c r="O3" s="31"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="32" t="s">
+      <c r="A4" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -2252,8 +2273,8 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
+      <c r="N5" s="35"/>
+      <c r="O5" s="35"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2292,11 +2313,11 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="M6" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -2505,7 +2526,7 @@
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>27</v>
@@ -2542,7 +2563,7 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>27</v>
@@ -2579,7 +2600,7 @@
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>27</v>
@@ -2616,7 +2637,7 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>27</v>
@@ -2700,22 +2721,22 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-      <c r="G22" s="24"/>
-      <c r="H22" s="24"/>
-      <c r="I22" s="24"/>
-      <c r="J22" s="24"/>
-      <c r="K22" s="24"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="24"/>
-      <c r="N22" s="24"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2724,93 +2745,98 @@
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="25"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
+      <c r="B24" s="38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25"/>
-      <c r="J25" s="25"/>
-      <c r="K25" s="25"/>
-      <c r="L25" s="25"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="37"/>
-      <c r="D26" s="37"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
-      <c r="H26" s="37"/>
-      <c r="I26" s="37"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="36"/>
+      <c r="C27" s="28"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="28"/>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="25"/>
-      <c r="J28" s="25"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="25"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
small changes to sprint log
</commit_message>
<xml_diff>
--- a/SnakeGame/Documents/Backlog Doc.xlsx
+++ b/SnakeGame/Documents/Backlog Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justy\source\repos\SnakeGame\SnakeGame\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztllo\OneDrive\Documents\GitHub\SnakeGame\SnakeGame\SnakeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B8EE84-D433-4091-B6F4-D2AAE6146357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110E6FDE-4D1C-42D8-931C-E4725EB29A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="68">
   <si>
     <t>Time Spent</t>
   </si>
@@ -187,9 +187,6 @@
     <t>Start the framework of the snake by incorporating it into a class</t>
   </si>
   <si>
-    <t>On going</t>
-  </si>
-  <si>
     <t>Start the framework of the game loop by incorporating it into a class</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
   </si>
   <si>
     <t>Summary</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Not Completed</t>
@@ -470,6 +464,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -482,16 +486,12 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -514,12 +514,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -867,76 +861,76 @@
       <selection activeCell="C15" sqref="C15:L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="73.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="16" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="15" max="16" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="N1" s="22"/>
-      <c r="O1" s="22"/>
-      <c r="P1" s="22"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="26"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="27"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -986,7 +980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1026,7 +1020,7 @@
       </c>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1064,7 +1058,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1102,7 +1096,7 @@
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1144,7 +1138,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1192,137 +1186,137 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
+      <c r="J13" s="29"/>
+      <c r="K13" s="29"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="29"/>
+      <c r="N13" s="29"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
+      <c r="K14" s="24"/>
+      <c r="L14" s="24"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="29"/>
-      <c r="E15" s="29"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="29"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="25"/>
+      <c r="L15" s="25"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22"/>
+      <c r="J16" s="22"/>
+      <c r="K16" s="22"/>
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="22"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="22"/>
+      <c r="J18" s="22"/>
+      <c r="K18" s="22"/>
+      <c r="L18" s="22"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="22"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="22"/>
+      <c r="J19" s="22"/>
+      <c r="K19" s="22"/>
+      <c r="L19" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="A13:N13"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C18:L18"/>
-    <mergeCell ref="A1:P2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="A13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1346,26 +1340,26 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.109375" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+    <col min="8" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1381,64 +1375,64 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1452,10 +1446,10 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1492,13 +1486,13 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1544,10 +1538,10 @@
       <c r="O7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="26"/>
-      <c r="Q7" s="26"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1594,7 +1588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1.2</v>
       </c>
@@ -1637,7 +1631,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1.2</v>
       </c>
@@ -1680,12 +1674,12 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1.2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C11" s="4">
         <v>1</v>
@@ -1725,12 +1719,12 @@
       </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1.3</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -1772,12 +1766,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1.3</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C13" s="4">
         <v>1</v>
@@ -1803,11 +1797,9 @@
       <c r="J13" s="3">
         <v>15</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="K13" s="4"/>
       <c r="L13" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>27</v>
@@ -1817,12 +1809,12 @@
       </c>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1.3</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" s="4">
         <v>1</v>
@@ -1848,11 +1840,9 @@
       <c r="J14" s="3">
         <v>15</v>
       </c>
-      <c r="K14" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="K14" s="4"/>
       <c r="L14" s="3" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>27</v>
@@ -1862,12 +1852,12 @@
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1.3</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3">
         <v>1</v>
@@ -1895,7 +1885,7 @@
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>27</v>
@@ -1905,12 +1895,12 @@
       </c>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1.3</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3">
         <v>1</v>
@@ -1938,7 +1928,7 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>27</v>
@@ -1948,7 +1938,7 @@
       </c>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1965,7 +1955,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1982,7 +1972,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -2027,126 +2017,132 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C23" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="C27:L27"/>
     <mergeCell ref="C28:L28"/>
     <mergeCell ref="A22:N22"/>
@@ -2154,12 +2150,6 @@
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C25:L25"/>
     <mergeCell ref="C26:L26"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2171,22 +2161,22 @@
   <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2202,64 +2192,64 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="32" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="33"/>
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="33"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="34" t="s">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="37"/>
+      <c r="I4" s="37"/>
+      <c r="J4" s="37"/>
+      <c r="K4" s="37"/>
+      <c r="L4" s="37"/>
+      <c r="M4" s="37"/>
+      <c r="N4" s="37"/>
+      <c r="O4" s="37"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -2273,10 +2263,10 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="35"/>
-      <c r="O5" s="35"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N5" s="37"/>
+      <c r="O5" s="37"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -2313,13 +2303,13 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2336,7 +2326,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -2353,12 +2343,12 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2.2000000000000002</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C9" s="4">
         <v>2</v>
@@ -2373,7 +2363,7 @@
         <v>15</v>
       </c>
       <c r="G9" s="3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H9" s="3">
         <v>0</v>
@@ -2382,7 +2372,7 @@
         <v>0</v>
       </c>
       <c r="J9" s="3">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="K9" s="5">
         <v>43763</v>
@@ -2400,12 +2390,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2.2000000000000002</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
@@ -2426,10 +2416,10 @@
         <v>10</v>
       </c>
       <c r="I10" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J10" s="3">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K10" s="5">
         <v>43766</v>
@@ -2447,12 +2437,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2.2000000000000002</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="4">
         <v>2</v>
@@ -2494,12 +2484,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C12" s="3">
         <v>2</v>
@@ -2517,13 +2507,13 @@
         <v>0</v>
       </c>
       <c r="H12" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="I12" s="3">
         <v>5</v>
       </c>
       <c r="J12" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="K12" s="5">
         <v>43775</v>
@@ -2541,12 +2531,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C13" s="4">
         <v>2</v>
@@ -2576,7 +2566,7 @@
         <v>0</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>27</v>
@@ -2588,12 +2578,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C14" s="4">
         <v>2</v>
@@ -2623,7 +2613,7 @@
         <v>0</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>27</v>
@@ -2635,12 +2625,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" s="3">
         <v>2</v>
@@ -2670,7 +2660,7 @@
         <v>0</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>27</v>
@@ -2682,12 +2672,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2.2999999999999998</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
@@ -2717,7 +2707,7 @@
         <v>0</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>27</v>
@@ -2729,7 +2719,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2746,7 +2736,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2763,7 +2753,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -2783,12 +2773,16 @@
         <v>120</v>
       </c>
       <c r="G19" s="11">
+        <v>15</v>
+      </c>
+      <c r="H19" s="11">
         <v>30</v>
       </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="I19" s="11">
+        <v>20</v>
+      </c>
       <c r="J19" s="11">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="3" t="s">
@@ -2804,123 +2798,123 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
-      <c r="L22" s="25"/>
-      <c r="M22" s="25"/>
-      <c r="N22" s="25"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C23" s="23" t="s">
+        <v>56</v>
+      </c>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+        <v>65</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="25"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="31"/>
+      <c r="K26" s="31"/>
+      <c r="L26" s="31"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="38"/>
-      <c r="D27" s="38"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="38"/>
-      <c r="G27" s="38"/>
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
-      <c r="J27" s="38"/>
-      <c r="K27" s="38"/>
-      <c r="L27" s="38"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="30"/>
+      <c r="J27" s="30"/>
+      <c r="K27" s="30"/>
+      <c r="L27" s="30"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="22"/>
+      <c r="G28" s="22"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="12">

</xml_diff>

<commit_message>
Sprint log 3 done
</commit_message>
<xml_diff>
--- a/SnakeGame/Documents/Backlog Doc.xlsx
+++ b/SnakeGame/Documents/Backlog Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\justy\source\repos\SnakeGame\SnakeGame\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztllo\OneDrive\Documents\GitHub\SnakeGame\SnakeGame\SnakeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C317A6-7DC7-4B5B-AC55-F8909B474426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62EBEA62-E571-477B-8909-7282FBF75C0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="75">
   <si>
     <t>Time Spent</t>
   </si>
@@ -243,13 +243,31 @@
   </si>
   <si>
     <t>Sprint 3 Backlog</t>
+  </si>
+  <si>
+    <t>Get movement working for the snake</t>
+  </si>
+  <si>
+    <t>Snake able to eat and grow in length</t>
+  </si>
+  <si>
+    <t>Clean up menu get it implemented</t>
+  </si>
+  <si>
+    <t>Work on game loop specifically end game</t>
+  </si>
+  <si>
+    <t>Polish</t>
+  </si>
+  <si>
+    <t>Get score implemented when snake eats (save it if possible)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -271,8 +289,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -318,6 +343,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -418,12 +448,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -468,23 +499,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -499,12 +516,16 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -529,10 +550,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="9" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -874,76 +920,76 @@
       <selection activeCell="C15" sqref="C15:L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="73.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="5" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="17.6640625" customWidth="1"/>
-    <col min="15" max="16" width="17.109375" customWidth="1"/>
+    <col min="2" max="2" width="73.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="5" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="15" max="16" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" s="31"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
-      <c r="I2" s="31"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="31"/>
-      <c r="L2" s="31"/>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="31"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26"/>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,7 +1039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1033,7 +1079,7 @@
       </c>
       <c r="P5" s="6"/>
     </row>
-    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1071,7 +1117,7 @@
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
     </row>
-    <row r="7" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1109,7 +1155,7 @@
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
     </row>
-    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1151,7 +1197,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>20</v>
       </c>
@@ -1199,137 +1245,137 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A13" s="33" t="s">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="34"/>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
-      <c r="G13" s="34"/>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="34"/>
-      <c r="L13" s="34"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="27"/>
-      <c r="L16" s="27"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C16" s="29"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="29"/>
+      <c r="I16" s="29"/>
+      <c r="J16" s="29"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="29"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+      <c r="I18" s="29"/>
+      <c r="J18" s="29"/>
+      <c r="K18" s="29"/>
+      <c r="L18" s="29"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="27"/>
-      <c r="L19" s="27"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="29"/>
+      <c r="J19" s="29"/>
+      <c r="K19" s="29"/>
+      <c r="L19" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:P2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="A13:N13"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C18:L18"/>
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="A13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1356,23 +1402,23 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="68.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="68.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
-    <col min="6" max="6" width="13.109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
     <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="9" width="7.6640625" customWidth="1"/>
-    <col min="10" max="10" width="6.44140625" customWidth="1"/>
-    <col min="11" max="11" width="12.44140625" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
-    <col min="13" max="13" width="20.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.109375" customWidth="1"/>
-    <col min="15" max="15" width="16.88671875" customWidth="1"/>
+    <col min="8" max="9" width="7.7109375" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="20.28515625" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" customWidth="1"/>
+    <col min="15" max="15" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1388,64 +1434,64 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -1459,10 +1505,10 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -1499,13 +1545,13 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1551,10 +1597,10 @@
       <c r="O7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1.1000000000000001</v>
       </c>
@@ -1601,7 +1647,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1.2</v>
       </c>
@@ -1644,7 +1690,7 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1.2</v>
       </c>
@@ -1687,7 +1733,7 @@
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1.2</v>
       </c>
@@ -1732,7 +1778,7 @@
       </c>
       <c r="O11" s="6"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1.3</v>
       </c>
@@ -1779,7 +1825,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>1.3</v>
       </c>
@@ -1822,7 +1868,7 @@
       </c>
       <c r="O13" s="6"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>1.3</v>
       </c>
@@ -1865,7 +1911,7 @@
       </c>
       <c r="O14" s="6"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1.3</v>
       </c>
@@ -1908,7 +1954,7 @@
       </c>
       <c r="O15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>1.3</v>
       </c>
@@ -1951,7 +1997,7 @@
       </c>
       <c r="O16" s="6"/>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1968,7 +2014,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1985,7 +2031,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -2030,132 +2076,126 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="C27:L27"/>
     <mergeCell ref="C28:L28"/>
     <mergeCell ref="A22:N22"/>
@@ -2163,6 +2203,12 @@
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C25:L25"/>
     <mergeCell ref="C26:L26"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2173,23 +2219,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E5EE9B2-143D-4149-A7B5-D0F1922FD7D1}">
   <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="64.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
     <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" customWidth="1"/>
-    <col min="14" max="14" width="18.88671875" customWidth="1"/>
-    <col min="15" max="15" width="17.88671875" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" customWidth="1"/>
+    <col min="14" max="14" width="18.85546875" customWidth="1"/>
+    <col min="15" max="15" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -2205,64 +2251,64 @@
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="39" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="41" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
+      <c r="O3" s="36"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -2276,10 +2322,10 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="42"/>
-      <c r="O5" s="42"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -2316,13 +2362,13 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="43" t="s">
+      <c r="M6" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="44"/>
-      <c r="O6" s="44"/>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -2339,7 +2385,7 @@
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
@@ -2356,7 +2402,7 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -2403,7 +2449,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -2450,7 +2496,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>2.2000000000000002</v>
       </c>
@@ -2497,7 +2543,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -2544,7 +2590,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -2591,7 +2637,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -2638,7 +2684,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -2685,7 +2731,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2.2999999999999998</v>
       </c>
@@ -2732,7 +2778,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -2749,7 +2795,7 @@
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -2766,7 +2812,7 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>20</v>
       </c>
@@ -2811,123 +2857,123 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A22" s="33" t="s">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="28"/>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="30" t="s">
+      <c r="C24" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="36"/>
-      <c r="D26" s="36"/>
-      <c r="E26" s="36"/>
-      <c r="F26" s="36"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="L26" s="42"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="35"/>
-      <c r="G27" s="35"/>
-      <c r="H27" s="35"/>
-      <c r="I27" s="35"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="35"/>
-      <c r="L27" s="35"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="41"/>
+      <c r="J27" s="41"/>
+      <c r="K27" s="41"/>
+      <c r="L27" s="41"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2953,79 +2999,81 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="53.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
-    <col min="13" max="13" width="18.21875" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" customWidth="1"/>
-    <col min="15" max="15" width="21.44140625" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" customWidth="1"/>
+    <col min="15" max="15" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
+      <c r="M1" s="34"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="42"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
@@ -3039,10 +3087,10 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-    </row>
-    <row r="5" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+    </row>
+    <row r="5" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>34</v>
       </c>
@@ -3079,29 +3127,39 @@
       <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="43" t="s">
+      <c r="M5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="44"/>
-      <c r="O5" s="44"/>
-    </row>
-    <row r="6" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="N5" s="40"/>
+      <c r="O5" s="40"/>
+    </row>
+    <row r="6" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>3.1</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
+        <v>3.2</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43780</v>
+      </c>
+      <c r="F6" s="3">
+        <v>15</v>
+      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
       <c r="K6" s="20"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M6" s="6" t="s">
         <v>28</v>
       </c>
@@ -3112,21 +3170,33 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>3.2</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43780</v>
+      </c>
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="20"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M7" s="6" t="s">
         <v>27</v>
       </c>
@@ -3137,21 +3207,33 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3.3</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43780</v>
+      </c>
+      <c r="F8" s="3">
+        <v>10</v>
+      </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="20"/>
-      <c r="L8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M8" s="6" t="s">
         <v>27</v>
       </c>
@@ -3162,21 +3244,33 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <v>3.4</v>
-      </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43780</v>
+      </c>
+      <c r="F9" s="3">
+        <v>10</v>
+      </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="20"/>
-      <c r="L9" s="3"/>
+      <c r="L9" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M9" s="6" t="s">
         <v>29</v>
       </c>
@@ -3187,21 +3281,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <v>3.5</v>
-      </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="3"/>
+        <v>3.2</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43780</v>
+      </c>
+      <c r="F10" s="3">
+        <v>15</v>
+      </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="20"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M10" s="6" t="s">
         <v>28</v>
       </c>
@@ -3212,21 +3318,33 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>3.6</v>
-      </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="3"/>
+        <v>3.4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3</v>
+      </c>
+      <c r="D11" s="3">
+        <v>3</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43780</v>
+      </c>
+      <c r="F11" s="3">
+        <v>10</v>
+      </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="20"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="M11" s="6" t="s">
         <v>29</v>
       </c>
@@ -3237,106 +3355,91 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="14">
-        <v>43738</v>
-      </c>
-      <c r="F12" s="11">
-        <v>120</v>
-      </c>
-      <c r="G12" s="11">
-        <v>0</v>
-      </c>
-      <c r="H12" s="11">
-        <v>0</v>
-      </c>
-      <c r="I12" s="11">
-        <v>0</v>
-      </c>
-      <c r="J12" s="11">
-        <v>0</v>
-      </c>
-      <c r="K12" s="11"/>
-      <c r="L12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="M12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O12" s="13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="33" t="s">
+      <c r="E12" s="46"/>
+      <c r="F12" s="45">
+        <v>70</v>
+      </c>
+      <c r="G12" s="45">
+        <v>0</v>
+      </c>
+      <c r="H12" s="45">
+        <v>0</v>
+      </c>
+      <c r="I12" s="45">
+        <v>0</v>
+      </c>
+      <c r="J12" s="45">
+        <v>0</v>
+      </c>
+      <c r="K12" s="45"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="43"/>
+      <c r="N12" s="43"/>
+      <c r="O12" s="43"/>
+    </row>
+    <row r="14" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
-      <c r="O14" s="22"/>
-    </row>
-    <row r="15" spans="1:15" s="23" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="24"/>
+    </row>
+    <row r="15" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="47" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="48" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="29"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A16" s="26">
-        <v>3.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="26">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="26">
-        <v>3.3</v>
-      </c>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="24"/>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="23"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="23"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
took out unneccasry zip and update backlog
</commit_message>
<xml_diff>
--- a/SnakeGame/Documents/Backlog Doc.xlsx
+++ b/SnakeGame/Documents/Backlog Doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztllo\OneDrive\Documents\GitHub\SnakeGame\SnakeGame\SnakeGame\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C734171-2D3C-4B89-93DC-85E44CFA5D21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF89CC79-EA16-4472-9D96-55791B35F94F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{0798A988-65CE-47D7-AD9B-BC4317E77DAB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="78">
   <si>
     <t>Time Spent</t>
   </si>
@@ -266,16 +266,10 @@
     <t>Complete</t>
   </si>
   <si>
-    <t>Still in the Works</t>
-  </si>
-  <si>
     <t>Making the snake grow when the snake eats food</t>
   </si>
   <si>
     <t>Still in the work, will be wrapped up for final demo</t>
-  </si>
-  <si>
-    <t>Still in the works</t>
   </si>
 </sst>
 </file>
@@ -534,16 +528,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="4" xfId="3" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="3" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -556,12 +540,16 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,6 +572,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
@@ -947,62 +941,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="32"/>
+      <c r="H1" s="32"/>
+      <c r="I1" s="32"/>
+      <c r="J1" s="32"/>
+      <c r="K1" s="32"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="32"/>
+      <c r="N1" s="32"/>
+      <c r="O1" s="32"/>
+      <c r="P1" s="32"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="36"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="36"/>
-      <c r="M2" s="36"/>
-      <c r="N2" s="36"/>
-      <c r="O2" s="36"/>
-      <c r="P2" s="36"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37"/>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37"/>
-      <c r="P3" s="37"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1261,22 +1255,22 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="38" t="s">
+      <c r="A13" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="35"/>
+      <c r="F13" s="35"/>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="35"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -1285,18 +1279,18 @@
       <c r="B14" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="33" t="s">
+      <c r="C14" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
-      <c r="J14" s="34"/>
-      <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1305,92 +1299,92 @@
       <c r="B15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2</v>
       </c>
-      <c r="C16" s="32"/>
-      <c r="D16" s="32"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="32"/>
-      <c r="H16" s="32"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>3</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>4</v>
       </c>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="32"/>
-      <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36"/>
+      <c r="E18" s="36"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36"/>
+      <c r="L18" s="36"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5</v>
       </c>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A1:P2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="L3:P3"/>
-    <mergeCell ref="A13:N13"/>
     <mergeCell ref="C19:L19"/>
     <mergeCell ref="C14:L14"/>
     <mergeCell ref="C15:L15"/>
     <mergeCell ref="C16:L16"/>
     <mergeCell ref="C17:L17"/>
     <mergeCell ref="C18:L18"/>
+    <mergeCell ref="A1:P2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="L3:P3"/>
+    <mergeCell ref="A13:N13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1450,61 +1444,61 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -1520,8 +1514,8 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -1560,11 +1554,11 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="48" t="s">
+      <c r="M6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
@@ -1612,8 +1606,8 @@
       <c r="O7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="32"/>
+      <c r="P7" s="36"/>
+      <c r="Q7" s="36"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -2092,22 +2086,22 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2116,18 +2110,18 @@
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2136,87 +2130,81 @@
       <c r="B24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="A2:O2"/>
-    <mergeCell ref="A3:O3"/>
-    <mergeCell ref="A4:O4"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="N5:O5"/>
     <mergeCell ref="C27:L27"/>
     <mergeCell ref="C28:L28"/>
     <mergeCell ref="A22:N22"/>
@@ -2224,6 +2212,12 @@
     <mergeCell ref="C24:L24"/>
     <mergeCell ref="C25:L25"/>
     <mergeCell ref="C26:L26"/>
+    <mergeCell ref="P7:Q7"/>
+    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A3:O3"/>
+    <mergeCell ref="A4:O4"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2267,61 +2261,61 @@
       <c r="N1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="40" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="L2" s="41"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="45"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="45"/>
-      <c r="H3" s="45"/>
-      <c r="I3" s="45"/>
-      <c r="J3" s="45"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="45"/>
-      <c r="M3" s="45"/>
-      <c r="N3" s="45"/>
-      <c r="O3" s="45"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
+      <c r="K3" s="43"/>
+      <c r="L3" s="43"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="43"/>
+      <c r="O3" s="43"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="47"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="47"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="45"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
@@ -2337,8 +2331,8 @@
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
-      <c r="N5" s="47"/>
-      <c r="O5" s="47"/>
+      <c r="N5" s="45"/>
+      <c r="O5" s="45"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2377,11 +2371,11 @@
       <c r="L6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="48" t="s">
+      <c r="M6" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="49"/>
-      <c r="O6" s="49"/>
+      <c r="N6" s="47"/>
+      <c r="O6" s="47"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
@@ -2873,22 +2867,22 @@
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A22" s="38" t="s">
+      <c r="A22" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="39"/>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
@@ -2897,18 +2891,18 @@
       <c r="B23" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="34"/>
-      <c r="E23" s="34"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="34"/>
-      <c r="H23" s="34"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
+      <c r="L23" s="38"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -2917,78 +2911,78 @@
       <c r="B24" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="35"/>
-      <c r="G24" s="35"/>
-      <c r="H24" s="35"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="39"/>
+      <c r="F24" s="39"/>
+      <c r="G24" s="39"/>
+      <c r="H24" s="39"/>
+      <c r="I24" s="39"/>
+      <c r="J24" s="39"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="39"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
-      <c r="C25" s="32"/>
-      <c r="D25" s="32"/>
-      <c r="E25" s="32"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
-      <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="36"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36"/>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="41"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
-      <c r="F27" s="40"/>
-      <c r="G27" s="40"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="40"/>
-      <c r="J27" s="40"/>
-      <c r="K27" s="40"/>
-      <c r="L27" s="40"/>
+      <c r="C27" s="48"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="48"/>
+      <c r="J27" s="48"/>
+      <c r="K27" s="48"/>
+      <c r="L27" s="48"/>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>5</v>
       </c>
-      <c r="C28" s="32"/>
-      <c r="D28" s="32"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
+      <c r="K28" s="36"/>
+      <c r="L28" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -3014,7 +3008,7 @@
   <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,61 +3026,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
+      <c r="J1" s="41"/>
+      <c r="K1" s="41"/>
+      <c r="L1" s="41"/>
+      <c r="M1" s="41"/>
+      <c r="N1" s="41"/>
+      <c r="O1" s="41"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="45"/>
-      <c r="I2" s="45"/>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="O2" s="45"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+      <c r="A3" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="47"/>
-      <c r="C3" s="47"/>
-      <c r="D3" s="47"/>
-      <c r="E3" s="47"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
+      <c r="D3" s="45"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="45"/>
+      <c r="H3" s="45"/>
+      <c r="I3" s="45"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="45"/>
+      <c r="L3" s="45"/>
+      <c r="M3" s="45"/>
+      <c r="N3" s="45"/>
+      <c r="O3" s="45"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
@@ -3102,8 +3096,8 @@
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="47"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="45"/>
     </row>
     <row r="5" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -3142,11 +3136,11 @@
       <c r="L5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M5" s="48" t="s">
+      <c r="M5" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="N5" s="49"/>
-      <c r="O5" s="49"/>
+      <c r="N5" s="47"/>
+      <c r="O5" s="47"/>
     </row>
     <row r="6" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
@@ -3226,11 +3220,11 @@
       <c r="J7" s="3">
         <v>18</v>
       </c>
-      <c r="K7" s="20" t="s">
-        <v>79</v>
+      <c r="K7" s="20">
+        <v>43802</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>27</v>
@@ -3466,22 +3460,22 @@
       <c r="O12" s="25"/>
     </row>
     <row r="14" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
       <c r="O14" s="24"/>
     </row>
     <row r="15" spans="1:15" s="22" customFormat="1" x14ac:dyDescent="0.25">
@@ -3512,10 +3506,10 @@
         <v>3.2</v>
       </c>
       <c r="B16" t="s">
+        <v>76</v>
+      </c>
+      <c r="C16" t="s">
         <v>77</v>
-      </c>
-      <c r="C16" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>